<commit_message>
add angular-filter, add projects and admin panel
</commit_message>
<xml_diff>
--- a/Project/IssueTracingSystem/app/app/JS-Frameworks-Self-Evaluation-Protocol.xlsx
+++ b/Project/IssueTracingSystem/app/app/JS-Frameworks-Self-Evaluation-Protocol.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SoftUni\AngularJS\Project IssueTracker\AngularJS\Project\IssueTracingSystem\app\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SoftUni\AngularJS Homework chek\AngularJS.git\trunk\Project\IssueTracingSystem\app\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -379,8 +379,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Нормален" xfId="0" builtinId="0"/>
-    <cellStyle name="Хипервръзка" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -396,9 +396,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема на Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Оffice">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -436,7 +436,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Оffice">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -508,7 +508,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Оffice">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -660,8 +660,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,7 +736,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>16</v>
@@ -748,7 +748,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>16</v>
@@ -828,7 +828,7 @@
         <v>21</v>
       </c>
       <c r="C16" s="4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D16" s="4">
         <v>10</v>
@@ -971,7 +971,9 @@
       <c r="B29" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="6"/>
+      <c r="C29" s="6">
+        <v>10</v>
+      </c>
       <c r="D29" s="6">
         <v>10</v>
       </c>
@@ -981,7 +983,9 @@
       <c r="B30" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="6"/>
+      <c r="C30" s="6">
+        <v>15</v>
+      </c>
       <c r="D30" s="6">
         <v>15</v>
       </c>
@@ -1003,7 +1007,7 @@
       </c>
       <c r="C32" s="10">
         <f>SUM(C6:C31)</f>
-        <v>229</v>
+        <v>251</v>
       </c>
       <c r="D32" s="10">
         <v>330</v>

</xml_diff>